<commit_message>
getting some sort of results...
</commit_message>
<xml_diff>
--- a/FR_Input.xlsx
+++ b/FR_Input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="0" windowWidth="17900" windowHeight="17540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="560" yWindow="0" windowWidth="19020" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Reg_Input" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="54">
   <si>
     <t>Fish</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Zoops</t>
-  </si>
-  <si>
-    <t>Phyto</t>
-  </si>
-  <si>
     <t>Weight (kg)</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>Dissolved oxygen saturation</t>
   </si>
   <si>
-    <t>DOC–octanol proportionality constant (deafult = .08)</t>
-  </si>
-  <si>
     <t>DOC–octanol proportionality constant (deafult = .35)</t>
   </si>
   <si>
@@ -129,18 +120,6 @@
     <t>Concentration in Sediment (g/Kg)</t>
   </si>
   <si>
-    <t>Disequilbrium factor of Disolved Organic Carbon</t>
-  </si>
-  <si>
-    <t>Disequilbrium factor of Particulate Organic Carbon</t>
-  </si>
-  <si>
-    <t>Total Concentration in Water (g/L)</t>
-  </si>
-  <si>
-    <t>Dissolved Concentration in Water (g/L)</t>
-  </si>
-  <si>
     <t>The Pond</t>
   </si>
   <si>
@@ -172,6 +151,39 @@
   </si>
   <si>
     <t>Growth Rate Iif known) (d^-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Water Tempature (°C)</t>
+  </si>
+  <si>
+    <t>POC–octanol proportionality constant (deafult = .08)</t>
+  </si>
+  <si>
+    <t>Extra Bad Chemical</t>
+  </si>
+  <si>
+    <t>Total Concentration in Water (g/L) (if avaliable)</t>
+  </si>
+  <si>
+    <t>Dissolved Concentration in Water (g/L) (if avaliable)</t>
+  </si>
+  <si>
+    <t>Disequilbrium factor of Disolved Organic Carbon (if avaliable)</t>
+  </si>
+  <si>
+    <t>Disequilbrium factor of Particulate Organic Carbon (if avaliable)</t>
+  </si>
+  <si>
+    <t>Fraction Pore Water Ventilated (deafult = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Concentration in Water (g/L) </t>
+  </si>
+  <si>
+    <t>Red Fish</t>
   </si>
 </sst>
 </file>
@@ -360,7 +372,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -412,8 +424,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -428,10 +452,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -447,8 +468,12 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -474,6 +499,12 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -499,6 +530,12 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -830,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -842,7 +879,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="11" customFormat="1" ht="23">
       <c r="A1" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -853,72 +890,74 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2">
-        <v>0.3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.4</v>
+      <c r="A4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="22">
+        <v>2.2000000000000001E-6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="2">
-        <v>2</v>
+      <c r="A5" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="23">
+        <v>5.4000000000000002E-7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="23">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="23">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="23">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="23"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="23"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" ht="23">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="B11" s="23"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6"/>
@@ -933,27 +972,27 @@
       <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="6"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="6"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="17"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="18"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="18"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="6"/>
     </row>
   </sheetData>
@@ -969,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -983,7 +1022,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1" ht="23">
       <c r="A1" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
@@ -991,31 +1030,31 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2">
         <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="25" t="s">
-        <v>37</v>
+      <c r="A5" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="B5" s="2">
         <v>0.1</v>
@@ -1023,7 +1062,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2">
         <v>0.02</v>
@@ -1031,22 +1070,77 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="23">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.05</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1061,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:HP36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1079,7 +1173,7 @@
     <col min="27" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="9" customFormat="1" ht="23">
+    <row r="1" spans="1:224" s="9" customFormat="1" ht="23">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1118,25 +1212,223 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
-    </row>
-    <row r="2" spans="1:26" s="5" customFormat="1">
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="4"/>
+      <c r="AL1" s="4"/>
+      <c r="AM1" s="4"/>
+      <c r="AN1" s="4"/>
+      <c r="AO1" s="4"/>
+      <c r="AP1" s="4"/>
+      <c r="AQ1" s="4"/>
+      <c r="AR1" s="4"/>
+      <c r="AS1" s="4"/>
+      <c r="AT1" s="4"/>
+      <c r="AU1" s="4"/>
+      <c r="AV1" s="4"/>
+      <c r="AW1" s="4"/>
+      <c r="AX1" s="4"/>
+      <c r="AY1" s="4"/>
+      <c r="AZ1" s="4"/>
+      <c r="BA1" s="4"/>
+      <c r="BB1" s="4"/>
+      <c r="BC1" s="4"/>
+      <c r="BD1" s="4"/>
+      <c r="BE1" s="4"/>
+      <c r="BF1" s="4"/>
+      <c r="BG1" s="4"/>
+      <c r="BH1" s="4"/>
+      <c r="BI1" s="4"/>
+      <c r="BJ1" s="4"/>
+      <c r="BK1" s="4"/>
+      <c r="BL1" s="4"/>
+      <c r="BM1" s="4"/>
+      <c r="BN1" s="4"/>
+      <c r="BO1" s="4"/>
+      <c r="BP1" s="4"/>
+      <c r="BQ1" s="4"/>
+      <c r="BR1" s="4"/>
+      <c r="BS1" s="4"/>
+      <c r="BT1" s="4"/>
+      <c r="BU1" s="4"/>
+      <c r="BV1" s="4"/>
+      <c r="BW1" s="4"/>
+      <c r="BX1" s="4"/>
+      <c r="BY1" s="4"/>
+      <c r="BZ1" s="4"/>
+      <c r="CA1" s="4"/>
+      <c r="CB1" s="4"/>
+      <c r="CC1" s="4"/>
+      <c r="CD1" s="4"/>
+      <c r="CE1" s="4"/>
+      <c r="CF1" s="4"/>
+      <c r="CG1" s="4"/>
+      <c r="CH1" s="4"/>
+      <c r="CI1" s="4"/>
+      <c r="CJ1" s="4"/>
+      <c r="CK1" s="4"/>
+      <c r="CL1" s="4"/>
+      <c r="CM1" s="4"/>
+      <c r="CN1" s="4"/>
+      <c r="CO1" s="4"/>
+      <c r="CP1" s="4"/>
+      <c r="CQ1" s="4"/>
+      <c r="CR1" s="4"/>
+      <c r="CS1" s="4"/>
+      <c r="CT1" s="4"/>
+      <c r="CU1" s="4"/>
+      <c r="CV1" s="4"/>
+      <c r="CW1" s="4"/>
+      <c r="CX1" s="4"/>
+      <c r="CY1" s="4"/>
+      <c r="CZ1" s="4"/>
+      <c r="DA1" s="4"/>
+      <c r="DB1" s="4"/>
+      <c r="DC1" s="4"/>
+      <c r="DD1" s="4"/>
+      <c r="DE1" s="4"/>
+      <c r="DF1" s="4"/>
+      <c r="DG1" s="4"/>
+      <c r="DH1" s="4"/>
+      <c r="DI1" s="4"/>
+      <c r="DJ1" s="4"/>
+      <c r="DK1" s="4"/>
+      <c r="DL1" s="4"/>
+      <c r="DM1" s="4"/>
+      <c r="DN1" s="4"/>
+      <c r="DO1" s="4"/>
+      <c r="DP1" s="4"/>
+      <c r="DQ1" s="4"/>
+      <c r="DR1" s="4"/>
+      <c r="DS1" s="4"/>
+      <c r="DT1" s="4"/>
+      <c r="DU1" s="4"/>
+      <c r="DV1" s="4"/>
+      <c r="DW1" s="4"/>
+      <c r="DX1" s="4"/>
+      <c r="DY1" s="4"/>
+      <c r="DZ1" s="4"/>
+      <c r="EA1" s="4"/>
+      <c r="EB1" s="4"/>
+      <c r="EC1" s="4"/>
+      <c r="ED1" s="4"/>
+      <c r="EE1" s="4"/>
+      <c r="EF1" s="4"/>
+      <c r="EG1" s="4"/>
+      <c r="EH1" s="4"/>
+      <c r="EI1" s="4"/>
+      <c r="EJ1" s="4"/>
+      <c r="EK1" s="4"/>
+      <c r="EL1" s="4"/>
+      <c r="EM1" s="4"/>
+      <c r="EN1" s="4"/>
+      <c r="EO1" s="4"/>
+      <c r="EP1" s="4"/>
+      <c r="EQ1" s="4"/>
+      <c r="ER1" s="4"/>
+      <c r="ES1" s="4"/>
+      <c r="ET1" s="4"/>
+      <c r="EU1" s="4"/>
+      <c r="EV1" s="4"/>
+      <c r="EW1" s="4"/>
+      <c r="EX1" s="4"/>
+      <c r="EY1" s="4"/>
+      <c r="EZ1" s="4"/>
+      <c r="FA1" s="4"/>
+      <c r="FB1" s="4"/>
+      <c r="FC1" s="4"/>
+      <c r="FD1" s="4"/>
+      <c r="FE1" s="4"/>
+      <c r="FF1" s="4"/>
+      <c r="FG1" s="4"/>
+      <c r="FH1" s="4"/>
+      <c r="FI1" s="4"/>
+      <c r="FJ1" s="4"/>
+      <c r="FK1" s="4"/>
+      <c r="FL1" s="4"/>
+      <c r="FM1" s="4"/>
+      <c r="FN1" s="4"/>
+      <c r="FO1" s="4"/>
+      <c r="FP1" s="4"/>
+      <c r="FQ1" s="4"/>
+      <c r="FR1" s="4"/>
+      <c r="FS1" s="4"/>
+      <c r="FT1" s="4"/>
+      <c r="FU1" s="4"/>
+      <c r="FV1" s="4"/>
+      <c r="FW1" s="4"/>
+      <c r="FX1" s="4"/>
+      <c r="FY1" s="4"/>
+      <c r="FZ1" s="4"/>
+      <c r="GA1" s="4"/>
+      <c r="GB1" s="4"/>
+      <c r="GC1" s="4"/>
+      <c r="GD1" s="4"/>
+      <c r="GE1" s="4"/>
+      <c r="GF1" s="4"/>
+      <c r="GG1" s="4"/>
+      <c r="GH1" s="4"/>
+      <c r="GI1" s="4"/>
+      <c r="GJ1" s="4"/>
+      <c r="GK1" s="4"/>
+      <c r="GL1" s="4"/>
+      <c r="GM1" s="4"/>
+      <c r="GN1" s="4"/>
+      <c r="GO1" s="4"/>
+      <c r="GP1" s="4"/>
+      <c r="GQ1" s="4"/>
+      <c r="GR1" s="4"/>
+      <c r="GS1" s="4"/>
+      <c r="GT1" s="4"/>
+      <c r="GU1" s="4"/>
+      <c r="GV1" s="4"/>
+      <c r="GW1" s="4"/>
+      <c r="GX1" s="4"/>
+      <c r="GY1" s="4"/>
+      <c r="GZ1" s="4"/>
+      <c r="HA1" s="4"/>
+      <c r="HB1" s="4"/>
+      <c r="HC1" s="4"/>
+      <c r="HD1" s="4"/>
+      <c r="HE1" s="4"/>
+      <c r="HF1" s="4"/>
+      <c r="HG1" s="4"/>
+      <c r="HH1" s="4"/>
+      <c r="HI1" s="4"/>
+      <c r="HJ1" s="4"/>
+      <c r="HK1" s="4"/>
+      <c r="HL1" s="4"/>
+      <c r="HM1" s="4"/>
+      <c r="HN1" s="4"/>
+      <c r="HO1" s="4"/>
+      <c r="HP1" s="4"/>
+    </row>
+    <row r="2" spans="1:224" s="5" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -1158,22 +1450,220 @@
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
-    </row>
-    <row r="3" spans="1:26" s="5" customFormat="1">
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
+      <c r="AM2" s="6"/>
+      <c r="AN2" s="6"/>
+      <c r="AO2" s="6"/>
+      <c r="AP2" s="6"/>
+      <c r="AQ2" s="6"/>
+      <c r="AR2" s="6"/>
+      <c r="AS2" s="6"/>
+      <c r="AT2" s="6"/>
+      <c r="AU2" s="6"/>
+      <c r="AV2" s="6"/>
+      <c r="AW2" s="6"/>
+      <c r="AX2" s="6"/>
+      <c r="AY2" s="6"/>
+      <c r="AZ2" s="6"/>
+      <c r="BA2" s="6"/>
+      <c r="BB2" s="6"/>
+      <c r="BC2" s="6"/>
+      <c r="BD2" s="6"/>
+      <c r="BE2" s="6"/>
+      <c r="BF2" s="6"/>
+      <c r="BG2" s="6"/>
+      <c r="BH2" s="6"/>
+      <c r="BI2" s="6"/>
+      <c r="BJ2" s="6"/>
+      <c r="BK2" s="6"/>
+      <c r="BL2" s="6"/>
+      <c r="BM2" s="6"/>
+      <c r="BN2" s="6"/>
+      <c r="BO2" s="6"/>
+      <c r="BP2" s="6"/>
+      <c r="BQ2" s="6"/>
+      <c r="BR2" s="6"/>
+      <c r="BS2" s="6"/>
+      <c r="BT2" s="6"/>
+      <c r="BU2" s="6"/>
+      <c r="BV2" s="6"/>
+      <c r="BW2" s="6"/>
+      <c r="BX2" s="6"/>
+      <c r="BY2" s="6"/>
+      <c r="BZ2" s="6"/>
+      <c r="CA2" s="6"/>
+      <c r="CB2" s="6"/>
+      <c r="CC2" s="6"/>
+      <c r="CD2" s="6"/>
+      <c r="CE2" s="6"/>
+      <c r="CF2" s="6"/>
+      <c r="CG2" s="6"/>
+      <c r="CH2" s="6"/>
+      <c r="CI2" s="6"/>
+      <c r="CJ2" s="6"/>
+      <c r="CK2" s="6"/>
+      <c r="CL2" s="6"/>
+      <c r="CM2" s="6"/>
+      <c r="CN2" s="6"/>
+      <c r="CO2" s="6"/>
+      <c r="CP2" s="6"/>
+      <c r="CQ2" s="6"/>
+      <c r="CR2" s="6"/>
+      <c r="CS2" s="6"/>
+      <c r="CT2" s="6"/>
+      <c r="CU2" s="6"/>
+      <c r="CV2" s="6"/>
+      <c r="CW2" s="6"/>
+      <c r="CX2" s="6"/>
+      <c r="CY2" s="6"/>
+      <c r="CZ2" s="6"/>
+      <c r="DA2" s="6"/>
+      <c r="DB2" s="6"/>
+      <c r="DC2" s="6"/>
+      <c r="DD2" s="6"/>
+      <c r="DE2" s="6"/>
+      <c r="DF2" s="6"/>
+      <c r="DG2" s="6"/>
+      <c r="DH2" s="6"/>
+      <c r="DI2" s="6"/>
+      <c r="DJ2" s="6"/>
+      <c r="DK2" s="6"/>
+      <c r="DL2" s="6"/>
+      <c r="DM2" s="6"/>
+      <c r="DN2" s="6"/>
+      <c r="DO2" s="6"/>
+      <c r="DP2" s="6"/>
+      <c r="DQ2" s="6"/>
+      <c r="DR2" s="6"/>
+      <c r="DS2" s="6"/>
+      <c r="DT2" s="6"/>
+      <c r="DU2" s="6"/>
+      <c r="DV2" s="6"/>
+      <c r="DW2" s="6"/>
+      <c r="DX2" s="6"/>
+      <c r="DY2" s="6"/>
+      <c r="DZ2" s="6"/>
+      <c r="EA2" s="6"/>
+      <c r="EB2" s="6"/>
+      <c r="EC2" s="6"/>
+      <c r="ED2" s="6"/>
+      <c r="EE2" s="6"/>
+      <c r="EF2" s="6"/>
+      <c r="EG2" s="6"/>
+      <c r="EH2" s="6"/>
+      <c r="EI2" s="6"/>
+      <c r="EJ2" s="6"/>
+      <c r="EK2" s="6"/>
+      <c r="EL2" s="6"/>
+      <c r="EM2" s="6"/>
+      <c r="EN2" s="6"/>
+      <c r="EO2" s="6"/>
+      <c r="EP2" s="6"/>
+      <c r="EQ2" s="6"/>
+      <c r="ER2" s="6"/>
+      <c r="ES2" s="6"/>
+      <c r="ET2" s="6"/>
+      <c r="EU2" s="6"/>
+      <c r="EV2" s="6"/>
+      <c r="EW2" s="6"/>
+      <c r="EX2" s="6"/>
+      <c r="EY2" s="6"/>
+      <c r="EZ2" s="6"/>
+      <c r="FA2" s="6"/>
+      <c r="FB2" s="6"/>
+      <c r="FC2" s="6"/>
+      <c r="FD2" s="6"/>
+      <c r="FE2" s="6"/>
+      <c r="FF2" s="6"/>
+      <c r="FG2" s="6"/>
+      <c r="FH2" s="6"/>
+      <c r="FI2" s="6"/>
+      <c r="FJ2" s="6"/>
+      <c r="FK2" s="6"/>
+      <c r="FL2" s="6"/>
+      <c r="FM2" s="6"/>
+      <c r="FN2" s="6"/>
+      <c r="FO2" s="6"/>
+      <c r="FP2" s="6"/>
+      <c r="FQ2" s="6"/>
+      <c r="FR2" s="6"/>
+      <c r="FS2" s="6"/>
+      <c r="FT2" s="6"/>
+      <c r="FU2" s="6"/>
+      <c r="FV2" s="6"/>
+      <c r="FW2" s="6"/>
+      <c r="FX2" s="6"/>
+      <c r="FY2" s="6"/>
+      <c r="FZ2" s="6"/>
+      <c r="GA2" s="6"/>
+      <c r="GB2" s="6"/>
+      <c r="GC2" s="6"/>
+      <c r="GD2" s="6"/>
+      <c r="GE2" s="6"/>
+      <c r="GF2" s="6"/>
+      <c r="GG2" s="6"/>
+      <c r="GH2" s="6"/>
+      <c r="GI2" s="6"/>
+      <c r="GJ2" s="6"/>
+      <c r="GK2" s="6"/>
+      <c r="GL2" s="6"/>
+      <c r="GM2" s="6"/>
+      <c r="GN2" s="6"/>
+      <c r="GO2" s="6"/>
+      <c r="GP2" s="6"/>
+      <c r="GQ2" s="6"/>
+      <c r="GR2" s="6"/>
+      <c r="GS2" s="6"/>
+      <c r="GT2" s="6"/>
+      <c r="GU2" s="6"/>
+      <c r="GV2" s="6"/>
+      <c r="GW2" s="6"/>
+      <c r="GX2" s="6"/>
+      <c r="GY2" s="6"/>
+      <c r="GZ2" s="6"/>
+      <c r="HA2" s="6"/>
+      <c r="HB2" s="6"/>
+      <c r="HC2" s="6"/>
+      <c r="HD2" s="6"/>
+      <c r="HE2" s="6"/>
+      <c r="HF2" s="6"/>
+      <c r="HG2" s="6"/>
+      <c r="HH2" s="6"/>
+      <c r="HI2" s="6"/>
+      <c r="HJ2" s="6"/>
+      <c r="HK2" s="6"/>
+      <c r="HL2" s="6"/>
+      <c r="HM2" s="6"/>
+      <c r="HN2" s="6"/>
+      <c r="HO2" s="6"/>
+      <c r="HP2" s="6"/>
+    </row>
+    <row r="3" spans="1:224" s="5" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2">
         <v>0.1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2">
         <v>0.01</v>
@@ -1198,24 +1688,222 @@
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
-    </row>
-    <row r="4" spans="1:26" s="5" customFormat="1">
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" s="6"/>
+      <c r="AM3" s="6"/>
+      <c r="AN3" s="6"/>
+      <c r="AO3" s="6"/>
+      <c r="AP3" s="6"/>
+      <c r="AQ3" s="6"/>
+      <c r="AR3" s="6"/>
+      <c r="AS3" s="6"/>
+      <c r="AT3" s="6"/>
+      <c r="AU3" s="6"/>
+      <c r="AV3" s="6"/>
+      <c r="AW3" s="6"/>
+      <c r="AX3" s="6"/>
+      <c r="AY3" s="6"/>
+      <c r="AZ3" s="6"/>
+      <c r="BA3" s="6"/>
+      <c r="BB3" s="6"/>
+      <c r="BC3" s="6"/>
+      <c r="BD3" s="6"/>
+      <c r="BE3" s="6"/>
+      <c r="BF3" s="6"/>
+      <c r="BG3" s="6"/>
+      <c r="BH3" s="6"/>
+      <c r="BI3" s="6"/>
+      <c r="BJ3" s="6"/>
+      <c r="BK3" s="6"/>
+      <c r="BL3" s="6"/>
+      <c r="BM3" s="6"/>
+      <c r="BN3" s="6"/>
+      <c r="BO3" s="6"/>
+      <c r="BP3" s="6"/>
+      <c r="BQ3" s="6"/>
+      <c r="BR3" s="6"/>
+      <c r="BS3" s="6"/>
+      <c r="BT3" s="6"/>
+      <c r="BU3" s="6"/>
+      <c r="BV3" s="6"/>
+      <c r="BW3" s="6"/>
+      <c r="BX3" s="6"/>
+      <c r="BY3" s="6"/>
+      <c r="BZ3" s="6"/>
+      <c r="CA3" s="6"/>
+      <c r="CB3" s="6"/>
+      <c r="CC3" s="6"/>
+      <c r="CD3" s="6"/>
+      <c r="CE3" s="6"/>
+      <c r="CF3" s="6"/>
+      <c r="CG3" s="6"/>
+      <c r="CH3" s="6"/>
+      <c r="CI3" s="6"/>
+      <c r="CJ3" s="6"/>
+      <c r="CK3" s="6"/>
+      <c r="CL3" s="6"/>
+      <c r="CM3" s="6"/>
+      <c r="CN3" s="6"/>
+      <c r="CO3" s="6"/>
+      <c r="CP3" s="6"/>
+      <c r="CQ3" s="6"/>
+      <c r="CR3" s="6"/>
+      <c r="CS3" s="6"/>
+      <c r="CT3" s="6"/>
+      <c r="CU3" s="6"/>
+      <c r="CV3" s="6"/>
+      <c r="CW3" s="6"/>
+      <c r="CX3" s="6"/>
+      <c r="CY3" s="6"/>
+      <c r="CZ3" s="6"/>
+      <c r="DA3" s="6"/>
+      <c r="DB3" s="6"/>
+      <c r="DC3" s="6"/>
+      <c r="DD3" s="6"/>
+      <c r="DE3" s="6"/>
+      <c r="DF3" s="6"/>
+      <c r="DG3" s="6"/>
+      <c r="DH3" s="6"/>
+      <c r="DI3" s="6"/>
+      <c r="DJ3" s="6"/>
+      <c r="DK3" s="6"/>
+      <c r="DL3" s="6"/>
+      <c r="DM3" s="6"/>
+      <c r="DN3" s="6"/>
+      <c r="DO3" s="6"/>
+      <c r="DP3" s="6"/>
+      <c r="DQ3" s="6"/>
+      <c r="DR3" s="6"/>
+      <c r="DS3" s="6"/>
+      <c r="DT3" s="6"/>
+      <c r="DU3" s="6"/>
+      <c r="DV3" s="6"/>
+      <c r="DW3" s="6"/>
+      <c r="DX3" s="6"/>
+      <c r="DY3" s="6"/>
+      <c r="DZ3" s="6"/>
+      <c r="EA3" s="6"/>
+      <c r="EB3" s="6"/>
+      <c r="EC3" s="6"/>
+      <c r="ED3" s="6"/>
+      <c r="EE3" s="6"/>
+      <c r="EF3" s="6"/>
+      <c r="EG3" s="6"/>
+      <c r="EH3" s="6"/>
+      <c r="EI3" s="6"/>
+      <c r="EJ3" s="6"/>
+      <c r="EK3" s="6"/>
+      <c r="EL3" s="6"/>
+      <c r="EM3" s="6"/>
+      <c r="EN3" s="6"/>
+      <c r="EO3" s="6"/>
+      <c r="EP3" s="6"/>
+      <c r="EQ3" s="6"/>
+      <c r="ER3" s="6"/>
+      <c r="ES3" s="6"/>
+      <c r="ET3" s="6"/>
+      <c r="EU3" s="6"/>
+      <c r="EV3" s="6"/>
+      <c r="EW3" s="6"/>
+      <c r="EX3" s="6"/>
+      <c r="EY3" s="6"/>
+      <c r="EZ3" s="6"/>
+      <c r="FA3" s="6"/>
+      <c r="FB3" s="6"/>
+      <c r="FC3" s="6"/>
+      <c r="FD3" s="6"/>
+      <c r="FE3" s="6"/>
+      <c r="FF3" s="6"/>
+      <c r="FG3" s="6"/>
+      <c r="FH3" s="6"/>
+      <c r="FI3" s="6"/>
+      <c r="FJ3" s="6"/>
+      <c r="FK3" s="6"/>
+      <c r="FL3" s="6"/>
+      <c r="FM3" s="6"/>
+      <c r="FN3" s="6"/>
+      <c r="FO3" s="6"/>
+      <c r="FP3" s="6"/>
+      <c r="FQ3" s="6"/>
+      <c r="FR3" s="6"/>
+      <c r="FS3" s="6"/>
+      <c r="FT3" s="6"/>
+      <c r="FU3" s="6"/>
+      <c r="FV3" s="6"/>
+      <c r="FW3" s="6"/>
+      <c r="FX3" s="6"/>
+      <c r="FY3" s="6"/>
+      <c r="FZ3" s="6"/>
+      <c r="GA3" s="6"/>
+      <c r="GB3" s="6"/>
+      <c r="GC3" s="6"/>
+      <c r="GD3" s="6"/>
+      <c r="GE3" s="6"/>
+      <c r="GF3" s="6"/>
+      <c r="GG3" s="6"/>
+      <c r="GH3" s="6"/>
+      <c r="GI3" s="6"/>
+      <c r="GJ3" s="6"/>
+      <c r="GK3" s="6"/>
+      <c r="GL3" s="6"/>
+      <c r="GM3" s="6"/>
+      <c r="GN3" s="6"/>
+      <c r="GO3" s="6"/>
+      <c r="GP3" s="6"/>
+      <c r="GQ3" s="6"/>
+      <c r="GR3" s="6"/>
+      <c r="GS3" s="6"/>
+      <c r="GT3" s="6"/>
+      <c r="GU3" s="6"/>
+      <c r="GV3" s="6"/>
+      <c r="GW3" s="6"/>
+      <c r="GX3" s="6"/>
+      <c r="GY3" s="6"/>
+      <c r="GZ3" s="6"/>
+      <c r="HA3" s="6"/>
+      <c r="HB3" s="6"/>
+      <c r="HC3" s="6"/>
+      <c r="HD3" s="6"/>
+      <c r="HE3" s="6"/>
+      <c r="HF3" s="6"/>
+      <c r="HG3" s="6"/>
+      <c r="HH3" s="6"/>
+      <c r="HI3" s="6"/>
+      <c r="HJ3" s="6"/>
+      <c r="HK3" s="6"/>
+      <c r="HL3" s="6"/>
+      <c r="HM3" s="6"/>
+      <c r="HN3" s="6"/>
+      <c r="HO3" s="6"/>
+      <c r="HP3" s="6"/>
+    </row>
+    <row r="4" spans="1:224" s="5" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>0.2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
         <v>0.1</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="23"/>
+      <c r="E4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="22"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -1236,24 +1924,222 @@
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" s="5" customFormat="1">
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="6"/>
+      <c r="AS4" s="6"/>
+      <c r="AT4" s="6"/>
+      <c r="AU4" s="6"/>
+      <c r="AV4" s="6"/>
+      <c r="AW4" s="6"/>
+      <c r="AX4" s="6"/>
+      <c r="AY4" s="6"/>
+      <c r="AZ4" s="6"/>
+      <c r="BA4" s="6"/>
+      <c r="BB4" s="6"/>
+      <c r="BC4" s="6"/>
+      <c r="BD4" s="6"/>
+      <c r="BE4" s="6"/>
+      <c r="BF4" s="6"/>
+      <c r="BG4" s="6"/>
+      <c r="BH4" s="6"/>
+      <c r="BI4" s="6"/>
+      <c r="BJ4" s="6"/>
+      <c r="BK4" s="6"/>
+      <c r="BL4" s="6"/>
+      <c r="BM4" s="6"/>
+      <c r="BN4" s="6"/>
+      <c r="BO4" s="6"/>
+      <c r="BP4" s="6"/>
+      <c r="BQ4" s="6"/>
+      <c r="BR4" s="6"/>
+      <c r="BS4" s="6"/>
+      <c r="BT4" s="6"/>
+      <c r="BU4" s="6"/>
+      <c r="BV4" s="6"/>
+      <c r="BW4" s="6"/>
+      <c r="BX4" s="6"/>
+      <c r="BY4" s="6"/>
+      <c r="BZ4" s="6"/>
+      <c r="CA4" s="6"/>
+      <c r="CB4" s="6"/>
+      <c r="CC4" s="6"/>
+      <c r="CD4" s="6"/>
+      <c r="CE4" s="6"/>
+      <c r="CF4" s="6"/>
+      <c r="CG4" s="6"/>
+      <c r="CH4" s="6"/>
+      <c r="CI4" s="6"/>
+      <c r="CJ4" s="6"/>
+      <c r="CK4" s="6"/>
+      <c r="CL4" s="6"/>
+      <c r="CM4" s="6"/>
+      <c r="CN4" s="6"/>
+      <c r="CO4" s="6"/>
+      <c r="CP4" s="6"/>
+      <c r="CQ4" s="6"/>
+      <c r="CR4" s="6"/>
+      <c r="CS4" s="6"/>
+      <c r="CT4" s="6"/>
+      <c r="CU4" s="6"/>
+      <c r="CV4" s="6"/>
+      <c r="CW4" s="6"/>
+      <c r="CX4" s="6"/>
+      <c r="CY4" s="6"/>
+      <c r="CZ4" s="6"/>
+      <c r="DA4" s="6"/>
+      <c r="DB4" s="6"/>
+      <c r="DC4" s="6"/>
+      <c r="DD4" s="6"/>
+      <c r="DE4" s="6"/>
+      <c r="DF4" s="6"/>
+      <c r="DG4" s="6"/>
+      <c r="DH4" s="6"/>
+      <c r="DI4" s="6"/>
+      <c r="DJ4" s="6"/>
+      <c r="DK4" s="6"/>
+      <c r="DL4" s="6"/>
+      <c r="DM4" s="6"/>
+      <c r="DN4" s="6"/>
+      <c r="DO4" s="6"/>
+      <c r="DP4" s="6"/>
+      <c r="DQ4" s="6"/>
+      <c r="DR4" s="6"/>
+      <c r="DS4" s="6"/>
+      <c r="DT4" s="6"/>
+      <c r="DU4" s="6"/>
+      <c r="DV4" s="6"/>
+      <c r="DW4" s="6"/>
+      <c r="DX4" s="6"/>
+      <c r="DY4" s="6"/>
+      <c r="DZ4" s="6"/>
+      <c r="EA4" s="6"/>
+      <c r="EB4" s="6"/>
+      <c r="EC4" s="6"/>
+      <c r="ED4" s="6"/>
+      <c r="EE4" s="6"/>
+      <c r="EF4" s="6"/>
+      <c r="EG4" s="6"/>
+      <c r="EH4" s="6"/>
+      <c r="EI4" s="6"/>
+      <c r="EJ4" s="6"/>
+      <c r="EK4" s="6"/>
+      <c r="EL4" s="6"/>
+      <c r="EM4" s="6"/>
+      <c r="EN4" s="6"/>
+      <c r="EO4" s="6"/>
+      <c r="EP4" s="6"/>
+      <c r="EQ4" s="6"/>
+      <c r="ER4" s="6"/>
+      <c r="ES4" s="6"/>
+      <c r="ET4" s="6"/>
+      <c r="EU4" s="6"/>
+      <c r="EV4" s="6"/>
+      <c r="EW4" s="6"/>
+      <c r="EX4" s="6"/>
+      <c r="EY4" s="6"/>
+      <c r="EZ4" s="6"/>
+      <c r="FA4" s="6"/>
+      <c r="FB4" s="6"/>
+      <c r="FC4" s="6"/>
+      <c r="FD4" s="6"/>
+      <c r="FE4" s="6"/>
+      <c r="FF4" s="6"/>
+      <c r="FG4" s="6"/>
+      <c r="FH4" s="6"/>
+      <c r="FI4" s="6"/>
+      <c r="FJ4" s="6"/>
+      <c r="FK4" s="6"/>
+      <c r="FL4" s="6"/>
+      <c r="FM4" s="6"/>
+      <c r="FN4" s="6"/>
+      <c r="FO4" s="6"/>
+      <c r="FP4" s="6"/>
+      <c r="FQ4" s="6"/>
+      <c r="FR4" s="6"/>
+      <c r="FS4" s="6"/>
+      <c r="FT4" s="6"/>
+      <c r="FU4" s="6"/>
+      <c r="FV4" s="6"/>
+      <c r="FW4" s="6"/>
+      <c r="FX4" s="6"/>
+      <c r="FY4" s="6"/>
+      <c r="FZ4" s="6"/>
+      <c r="GA4" s="6"/>
+      <c r="GB4" s="6"/>
+      <c r="GC4" s="6"/>
+      <c r="GD4" s="6"/>
+      <c r="GE4" s="6"/>
+      <c r="GF4" s="6"/>
+      <c r="GG4" s="6"/>
+      <c r="GH4" s="6"/>
+      <c r="GI4" s="6"/>
+      <c r="GJ4" s="6"/>
+      <c r="GK4" s="6"/>
+      <c r="GL4" s="6"/>
+      <c r="GM4" s="6"/>
+      <c r="GN4" s="6"/>
+      <c r="GO4" s="6"/>
+      <c r="GP4" s="6"/>
+      <c r="GQ4" s="6"/>
+      <c r="GR4" s="6"/>
+      <c r="GS4" s="6"/>
+      <c r="GT4" s="6"/>
+      <c r="GU4" s="6"/>
+      <c r="GV4" s="6"/>
+      <c r="GW4" s="6"/>
+      <c r="GX4" s="6"/>
+      <c r="GY4" s="6"/>
+      <c r="GZ4" s="6"/>
+      <c r="HA4" s="6"/>
+      <c r="HB4" s="6"/>
+      <c r="HC4" s="6"/>
+      <c r="HD4" s="6"/>
+      <c r="HE4" s="6"/>
+      <c r="HF4" s="6"/>
+      <c r="HG4" s="6"/>
+      <c r="HH4" s="6"/>
+      <c r="HI4" s="6"/>
+      <c r="HJ4" s="6"/>
+      <c r="HK4" s="6"/>
+      <c r="HL4" s="6"/>
+      <c r="HM4" s="6"/>
+      <c r="HN4" s="6"/>
+      <c r="HO4" s="6"/>
+      <c r="HP4" s="6"/>
+    </row>
+    <row r="5" spans="1:224" s="5" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>0.2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>0.3</v>
       </c>
-      <c r="E5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="24"/>
+      <c r="E5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="23"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1274,22 +2160,222 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" s="5" customFormat="1">
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="6"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
+      <c r="AR5" s="6"/>
+      <c r="AS5" s="6"/>
+      <c r="AT5" s="6"/>
+      <c r="AU5" s="6"/>
+      <c r="AV5" s="6"/>
+      <c r="AW5" s="6"/>
+      <c r="AX5" s="6"/>
+      <c r="AY5" s="6"/>
+      <c r="AZ5" s="6"/>
+      <c r="BA5" s="6"/>
+      <c r="BB5" s="6"/>
+      <c r="BC5" s="6"/>
+      <c r="BD5" s="6"/>
+      <c r="BE5" s="6"/>
+      <c r="BF5" s="6"/>
+      <c r="BG5" s="6"/>
+      <c r="BH5" s="6"/>
+      <c r="BI5" s="6"/>
+      <c r="BJ5" s="6"/>
+      <c r="BK5" s="6"/>
+      <c r="BL5" s="6"/>
+      <c r="BM5" s="6"/>
+      <c r="BN5" s="6"/>
+      <c r="BO5" s="6"/>
+      <c r="BP5" s="6"/>
+      <c r="BQ5" s="6"/>
+      <c r="BR5" s="6"/>
+      <c r="BS5" s="6"/>
+      <c r="BT5" s="6"/>
+      <c r="BU5" s="6"/>
+      <c r="BV5" s="6"/>
+      <c r="BW5" s="6"/>
+      <c r="BX5" s="6"/>
+      <c r="BY5" s="6"/>
+      <c r="BZ5" s="6"/>
+      <c r="CA5" s="6"/>
+      <c r="CB5" s="6"/>
+      <c r="CC5" s="6"/>
+      <c r="CD5" s="6"/>
+      <c r="CE5" s="6"/>
+      <c r="CF5" s="6"/>
+      <c r="CG5" s="6"/>
+      <c r="CH5" s="6"/>
+      <c r="CI5" s="6"/>
+      <c r="CJ5" s="6"/>
+      <c r="CK5" s="6"/>
+      <c r="CL5" s="6"/>
+      <c r="CM5" s="6"/>
+      <c r="CN5" s="6"/>
+      <c r="CO5" s="6"/>
+      <c r="CP5" s="6"/>
+      <c r="CQ5" s="6"/>
+      <c r="CR5" s="6"/>
+      <c r="CS5" s="6"/>
+      <c r="CT5" s="6"/>
+      <c r="CU5" s="6"/>
+      <c r="CV5" s="6"/>
+      <c r="CW5" s="6"/>
+      <c r="CX5" s="6"/>
+      <c r="CY5" s="6"/>
+      <c r="CZ5" s="6"/>
+      <c r="DA5" s="6"/>
+      <c r="DB5" s="6"/>
+      <c r="DC5" s="6"/>
+      <c r="DD5" s="6"/>
+      <c r="DE5" s="6"/>
+      <c r="DF5" s="6"/>
+      <c r="DG5" s="6"/>
+      <c r="DH5" s="6"/>
+      <c r="DI5" s="6"/>
+      <c r="DJ5" s="6"/>
+      <c r="DK5" s="6"/>
+      <c r="DL5" s="6"/>
+      <c r="DM5" s="6"/>
+      <c r="DN5" s="6"/>
+      <c r="DO5" s="6"/>
+      <c r="DP5" s="6"/>
+      <c r="DQ5" s="6"/>
+      <c r="DR5" s="6"/>
+      <c r="DS5" s="6"/>
+      <c r="DT5" s="6"/>
+      <c r="DU5" s="6"/>
+      <c r="DV5" s="6"/>
+      <c r="DW5" s="6"/>
+      <c r="DX5" s="6"/>
+      <c r="DY5" s="6"/>
+      <c r="DZ5" s="6"/>
+      <c r="EA5" s="6"/>
+      <c r="EB5" s="6"/>
+      <c r="EC5" s="6"/>
+      <c r="ED5" s="6"/>
+      <c r="EE5" s="6"/>
+      <c r="EF5" s="6"/>
+      <c r="EG5" s="6"/>
+      <c r="EH5" s="6"/>
+      <c r="EI5" s="6"/>
+      <c r="EJ5" s="6"/>
+      <c r="EK5" s="6"/>
+      <c r="EL5" s="6"/>
+      <c r="EM5" s="6"/>
+      <c r="EN5" s="6"/>
+      <c r="EO5" s="6"/>
+      <c r="EP5" s="6"/>
+      <c r="EQ5" s="6"/>
+      <c r="ER5" s="6"/>
+      <c r="ES5" s="6"/>
+      <c r="ET5" s="6"/>
+      <c r="EU5" s="6"/>
+      <c r="EV5" s="6"/>
+      <c r="EW5" s="6"/>
+      <c r="EX5" s="6"/>
+      <c r="EY5" s="6"/>
+      <c r="EZ5" s="6"/>
+      <c r="FA5" s="6"/>
+      <c r="FB5" s="6"/>
+      <c r="FC5" s="6"/>
+      <c r="FD5" s="6"/>
+      <c r="FE5" s="6"/>
+      <c r="FF5" s="6"/>
+      <c r="FG5" s="6"/>
+      <c r="FH5" s="6"/>
+      <c r="FI5" s="6"/>
+      <c r="FJ5" s="6"/>
+      <c r="FK5" s="6"/>
+      <c r="FL5" s="6"/>
+      <c r="FM5" s="6"/>
+      <c r="FN5" s="6"/>
+      <c r="FO5" s="6"/>
+      <c r="FP5" s="6"/>
+      <c r="FQ5" s="6"/>
+      <c r="FR5" s="6"/>
+      <c r="FS5" s="6"/>
+      <c r="FT5" s="6"/>
+      <c r="FU5" s="6"/>
+      <c r="FV5" s="6"/>
+      <c r="FW5" s="6"/>
+      <c r="FX5" s="6"/>
+      <c r="FY5" s="6"/>
+      <c r="FZ5" s="6"/>
+      <c r="GA5" s="6"/>
+      <c r="GB5" s="6"/>
+      <c r="GC5" s="6"/>
+      <c r="GD5" s="6"/>
+      <c r="GE5" s="6"/>
+      <c r="GF5" s="6"/>
+      <c r="GG5" s="6"/>
+      <c r="GH5" s="6"/>
+      <c r="GI5" s="6"/>
+      <c r="GJ5" s="6"/>
+      <c r="GK5" s="6"/>
+      <c r="GL5" s="6"/>
+      <c r="GM5" s="6"/>
+      <c r="GN5" s="6"/>
+      <c r="GO5" s="6"/>
+      <c r="GP5" s="6"/>
+      <c r="GQ5" s="6"/>
+      <c r="GR5" s="6"/>
+      <c r="GS5" s="6"/>
+      <c r="GT5" s="6"/>
+      <c r="GU5" s="6"/>
+      <c r="GV5" s="6"/>
+      <c r="GW5" s="6"/>
+      <c r="GX5" s="6"/>
+      <c r="GY5" s="6"/>
+      <c r="GZ5" s="6"/>
+      <c r="HA5" s="6"/>
+      <c r="HB5" s="6"/>
+      <c r="HC5" s="6"/>
+      <c r="HD5" s="6"/>
+      <c r="HE5" s="6"/>
+      <c r="HF5" s="6"/>
+      <c r="HG5" s="6"/>
+      <c r="HH5" s="6"/>
+      <c r="HI5" s="6"/>
+      <c r="HJ5" s="6"/>
+      <c r="HK5" s="6"/>
+      <c r="HL5" s="6"/>
+      <c r="HM5" s="6"/>
+      <c r="HN5" s="6"/>
+      <c r="HO5" s="6"/>
+      <c r="HP5" s="6"/>
+    </row>
+    <row r="6" spans="1:224" s="5" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>0.7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="D6" s="2">
         <v>0.2</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -1310,16 +2396,214 @@
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-    </row>
-    <row r="7" spans="1:26" s="5" customFormat="1">
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="6"/>
+      <c r="AM6" s="6"/>
+      <c r="AN6" s="6"/>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="6"/>
+      <c r="AQ6" s="6"/>
+      <c r="AR6" s="6"/>
+      <c r="AS6" s="6"/>
+      <c r="AT6" s="6"/>
+      <c r="AU6" s="6"/>
+      <c r="AV6" s="6"/>
+      <c r="AW6" s="6"/>
+      <c r="AX6" s="6"/>
+      <c r="AY6" s="6"/>
+      <c r="AZ6" s="6"/>
+      <c r="BA6" s="6"/>
+      <c r="BB6" s="6"/>
+      <c r="BC6" s="6"/>
+      <c r="BD6" s="6"/>
+      <c r="BE6" s="6"/>
+      <c r="BF6" s="6"/>
+      <c r="BG6" s="6"/>
+      <c r="BH6" s="6"/>
+      <c r="BI6" s="6"/>
+      <c r="BJ6" s="6"/>
+      <c r="BK6" s="6"/>
+      <c r="BL6" s="6"/>
+      <c r="BM6" s="6"/>
+      <c r="BN6" s="6"/>
+      <c r="BO6" s="6"/>
+      <c r="BP6" s="6"/>
+      <c r="BQ6" s="6"/>
+      <c r="BR6" s="6"/>
+      <c r="BS6" s="6"/>
+      <c r="BT6" s="6"/>
+      <c r="BU6" s="6"/>
+      <c r="BV6" s="6"/>
+      <c r="BW6" s="6"/>
+      <c r="BX6" s="6"/>
+      <c r="BY6" s="6"/>
+      <c r="BZ6" s="6"/>
+      <c r="CA6" s="6"/>
+      <c r="CB6" s="6"/>
+      <c r="CC6" s="6"/>
+      <c r="CD6" s="6"/>
+      <c r="CE6" s="6"/>
+      <c r="CF6" s="6"/>
+      <c r="CG6" s="6"/>
+      <c r="CH6" s="6"/>
+      <c r="CI6" s="6"/>
+      <c r="CJ6" s="6"/>
+      <c r="CK6" s="6"/>
+      <c r="CL6" s="6"/>
+      <c r="CM6" s="6"/>
+      <c r="CN6" s="6"/>
+      <c r="CO6" s="6"/>
+      <c r="CP6" s="6"/>
+      <c r="CQ6" s="6"/>
+      <c r="CR6" s="6"/>
+      <c r="CS6" s="6"/>
+      <c r="CT6" s="6"/>
+      <c r="CU6" s="6"/>
+      <c r="CV6" s="6"/>
+      <c r="CW6" s="6"/>
+      <c r="CX6" s="6"/>
+      <c r="CY6" s="6"/>
+      <c r="CZ6" s="6"/>
+      <c r="DA6" s="6"/>
+      <c r="DB6" s="6"/>
+      <c r="DC6" s="6"/>
+      <c r="DD6" s="6"/>
+      <c r="DE6" s="6"/>
+      <c r="DF6" s="6"/>
+      <c r="DG6" s="6"/>
+      <c r="DH6" s="6"/>
+      <c r="DI6" s="6"/>
+      <c r="DJ6" s="6"/>
+      <c r="DK6" s="6"/>
+      <c r="DL6" s="6"/>
+      <c r="DM6" s="6"/>
+      <c r="DN6" s="6"/>
+      <c r="DO6" s="6"/>
+      <c r="DP6" s="6"/>
+      <c r="DQ6" s="6"/>
+      <c r="DR6" s="6"/>
+      <c r="DS6" s="6"/>
+      <c r="DT6" s="6"/>
+      <c r="DU6" s="6"/>
+      <c r="DV6" s="6"/>
+      <c r="DW6" s="6"/>
+      <c r="DX6" s="6"/>
+      <c r="DY6" s="6"/>
+      <c r="DZ6" s="6"/>
+      <c r="EA6" s="6"/>
+      <c r="EB6" s="6"/>
+      <c r="EC6" s="6"/>
+      <c r="ED6" s="6"/>
+      <c r="EE6" s="6"/>
+      <c r="EF6" s="6"/>
+      <c r="EG6" s="6"/>
+      <c r="EH6" s="6"/>
+      <c r="EI6" s="6"/>
+      <c r="EJ6" s="6"/>
+      <c r="EK6" s="6"/>
+      <c r="EL6" s="6"/>
+      <c r="EM6" s="6"/>
+      <c r="EN6" s="6"/>
+      <c r="EO6" s="6"/>
+      <c r="EP6" s="6"/>
+      <c r="EQ6" s="6"/>
+      <c r="ER6" s="6"/>
+      <c r="ES6" s="6"/>
+      <c r="ET6" s="6"/>
+      <c r="EU6" s="6"/>
+      <c r="EV6" s="6"/>
+      <c r="EW6" s="6"/>
+      <c r="EX6" s="6"/>
+      <c r="EY6" s="6"/>
+      <c r="EZ6" s="6"/>
+      <c r="FA6" s="6"/>
+      <c r="FB6" s="6"/>
+      <c r="FC6" s="6"/>
+      <c r="FD6" s="6"/>
+      <c r="FE6" s="6"/>
+      <c r="FF6" s="6"/>
+      <c r="FG6" s="6"/>
+      <c r="FH6" s="6"/>
+      <c r="FI6" s="6"/>
+      <c r="FJ6" s="6"/>
+      <c r="FK6" s="6"/>
+      <c r="FL6" s="6"/>
+      <c r="FM6" s="6"/>
+      <c r="FN6" s="6"/>
+      <c r="FO6" s="6"/>
+      <c r="FP6" s="6"/>
+      <c r="FQ6" s="6"/>
+      <c r="FR6" s="6"/>
+      <c r="FS6" s="6"/>
+      <c r="FT6" s="6"/>
+      <c r="FU6" s="6"/>
+      <c r="FV6" s="6"/>
+      <c r="FW6" s="6"/>
+      <c r="FX6" s="6"/>
+      <c r="FY6" s="6"/>
+      <c r="FZ6" s="6"/>
+      <c r="GA6" s="6"/>
+      <c r="GB6" s="6"/>
+      <c r="GC6" s="6"/>
+      <c r="GD6" s="6"/>
+      <c r="GE6" s="6"/>
+      <c r="GF6" s="6"/>
+      <c r="GG6" s="6"/>
+      <c r="GH6" s="6"/>
+      <c r="GI6" s="6"/>
+      <c r="GJ6" s="6"/>
+      <c r="GK6" s="6"/>
+      <c r="GL6" s="6"/>
+      <c r="GM6" s="6"/>
+      <c r="GN6" s="6"/>
+      <c r="GO6" s="6"/>
+      <c r="GP6" s="6"/>
+      <c r="GQ6" s="6"/>
+      <c r="GR6" s="6"/>
+      <c r="GS6" s="6"/>
+      <c r="GT6" s="6"/>
+      <c r="GU6" s="6"/>
+      <c r="GV6" s="6"/>
+      <c r="GW6" s="6"/>
+      <c r="GX6" s="6"/>
+      <c r="GY6" s="6"/>
+      <c r="GZ6" s="6"/>
+      <c r="HA6" s="6"/>
+      <c r="HB6" s="6"/>
+      <c r="HC6" s="6"/>
+      <c r="HD6" s="6"/>
+      <c r="HE6" s="6"/>
+      <c r="HF6" s="6"/>
+      <c r="HG6" s="6"/>
+      <c r="HH6" s="6"/>
+      <c r="HI6" s="6"/>
+      <c r="HJ6" s="6"/>
+      <c r="HK6" s="6"/>
+      <c r="HL6" s="6"/>
+      <c r="HM6" s="6"/>
+      <c r="HN6" s="6"/>
+      <c r="HO6" s="6"/>
+      <c r="HP6" s="6"/>
+    </row>
+    <row r="7" spans="1:224" s="5" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="6"/>
@@ -1344,14 +2628,212 @@
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
-    </row>
-    <row r="8" spans="1:26" s="5" customFormat="1">
-      <c r="A8" s="19" t="s">
-        <v>15</v>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="6"/>
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="6"/>
+      <c r="AS7" s="6"/>
+      <c r="AT7" s="6"/>
+      <c r="AU7" s="6"/>
+      <c r="AV7" s="6"/>
+      <c r="AW7" s="6"/>
+      <c r="AX7" s="6"/>
+      <c r="AY7" s="6"/>
+      <c r="AZ7" s="6"/>
+      <c r="BA7" s="6"/>
+      <c r="BB7" s="6"/>
+      <c r="BC7" s="6"/>
+      <c r="BD7" s="6"/>
+      <c r="BE7" s="6"/>
+      <c r="BF7" s="6"/>
+      <c r="BG7" s="6"/>
+      <c r="BH7" s="6"/>
+      <c r="BI7" s="6"/>
+      <c r="BJ7" s="6"/>
+      <c r="BK7" s="6"/>
+      <c r="BL7" s="6"/>
+      <c r="BM7" s="6"/>
+      <c r="BN7" s="6"/>
+      <c r="BO7" s="6"/>
+      <c r="BP7" s="6"/>
+      <c r="BQ7" s="6"/>
+      <c r="BR7" s="6"/>
+      <c r="BS7" s="6"/>
+      <c r="BT7" s="6"/>
+      <c r="BU7" s="6"/>
+      <c r="BV7" s="6"/>
+      <c r="BW7" s="6"/>
+      <c r="BX7" s="6"/>
+      <c r="BY7" s="6"/>
+      <c r="BZ7" s="6"/>
+      <c r="CA7" s="6"/>
+      <c r="CB7" s="6"/>
+      <c r="CC7" s="6"/>
+      <c r="CD7" s="6"/>
+      <c r="CE7" s="6"/>
+      <c r="CF7" s="6"/>
+      <c r="CG7" s="6"/>
+      <c r="CH7" s="6"/>
+      <c r="CI7" s="6"/>
+      <c r="CJ7" s="6"/>
+      <c r="CK7" s="6"/>
+      <c r="CL7" s="6"/>
+      <c r="CM7" s="6"/>
+      <c r="CN7" s="6"/>
+      <c r="CO7" s="6"/>
+      <c r="CP7" s="6"/>
+      <c r="CQ7" s="6"/>
+      <c r="CR7" s="6"/>
+      <c r="CS7" s="6"/>
+      <c r="CT7" s="6"/>
+      <c r="CU7" s="6"/>
+      <c r="CV7" s="6"/>
+      <c r="CW7" s="6"/>
+      <c r="CX7" s="6"/>
+      <c r="CY7" s="6"/>
+      <c r="CZ7" s="6"/>
+      <c r="DA7" s="6"/>
+      <c r="DB7" s="6"/>
+      <c r="DC7" s="6"/>
+      <c r="DD7" s="6"/>
+      <c r="DE7" s="6"/>
+      <c r="DF7" s="6"/>
+      <c r="DG7" s="6"/>
+      <c r="DH7" s="6"/>
+      <c r="DI7" s="6"/>
+      <c r="DJ7" s="6"/>
+      <c r="DK7" s="6"/>
+      <c r="DL7" s="6"/>
+      <c r="DM7" s="6"/>
+      <c r="DN7" s="6"/>
+      <c r="DO7" s="6"/>
+      <c r="DP7" s="6"/>
+      <c r="DQ7" s="6"/>
+      <c r="DR7" s="6"/>
+      <c r="DS7" s="6"/>
+      <c r="DT7" s="6"/>
+      <c r="DU7" s="6"/>
+      <c r="DV7" s="6"/>
+      <c r="DW7" s="6"/>
+      <c r="DX7" s="6"/>
+      <c r="DY7" s="6"/>
+      <c r="DZ7" s="6"/>
+      <c r="EA7" s="6"/>
+      <c r="EB7" s="6"/>
+      <c r="EC7" s="6"/>
+      <c r="ED7" s="6"/>
+      <c r="EE7" s="6"/>
+      <c r="EF7" s="6"/>
+      <c r="EG7" s="6"/>
+      <c r="EH7" s="6"/>
+      <c r="EI7" s="6"/>
+      <c r="EJ7" s="6"/>
+      <c r="EK7" s="6"/>
+      <c r="EL7" s="6"/>
+      <c r="EM7" s="6"/>
+      <c r="EN7" s="6"/>
+      <c r="EO7" s="6"/>
+      <c r="EP7" s="6"/>
+      <c r="EQ7" s="6"/>
+      <c r="ER7" s="6"/>
+      <c r="ES7" s="6"/>
+      <c r="ET7" s="6"/>
+      <c r="EU7" s="6"/>
+      <c r="EV7" s="6"/>
+      <c r="EW7" s="6"/>
+      <c r="EX7" s="6"/>
+      <c r="EY7" s="6"/>
+      <c r="EZ7" s="6"/>
+      <c r="FA7" s="6"/>
+      <c r="FB7" s="6"/>
+      <c r="FC7" s="6"/>
+      <c r="FD7" s="6"/>
+      <c r="FE7" s="6"/>
+      <c r="FF7" s="6"/>
+      <c r="FG7" s="6"/>
+      <c r="FH7" s="6"/>
+      <c r="FI7" s="6"/>
+      <c r="FJ7" s="6"/>
+      <c r="FK7" s="6"/>
+      <c r="FL7" s="6"/>
+      <c r="FM7" s="6"/>
+      <c r="FN7" s="6"/>
+      <c r="FO7" s="6"/>
+      <c r="FP7" s="6"/>
+      <c r="FQ7" s="6"/>
+      <c r="FR7" s="6"/>
+      <c r="FS7" s="6"/>
+      <c r="FT7" s="6"/>
+      <c r="FU7" s="6"/>
+      <c r="FV7" s="6"/>
+      <c r="FW7" s="6"/>
+      <c r="FX7" s="6"/>
+      <c r="FY7" s="6"/>
+      <c r="FZ7" s="6"/>
+      <c r="GA7" s="6"/>
+      <c r="GB7" s="6"/>
+      <c r="GC7" s="6"/>
+      <c r="GD7" s="6"/>
+      <c r="GE7" s="6"/>
+      <c r="GF7" s="6"/>
+      <c r="GG7" s="6"/>
+      <c r="GH7" s="6"/>
+      <c r="GI7" s="6"/>
+      <c r="GJ7" s="6"/>
+      <c r="GK7" s="6"/>
+      <c r="GL7" s="6"/>
+      <c r="GM7" s="6"/>
+      <c r="GN7" s="6"/>
+      <c r="GO7" s="6"/>
+      <c r="GP7" s="6"/>
+      <c r="GQ7" s="6"/>
+      <c r="GR7" s="6"/>
+      <c r="GS7" s="6"/>
+      <c r="GT7" s="6"/>
+      <c r="GU7" s="6"/>
+      <c r="GV7" s="6"/>
+      <c r="GW7" s="6"/>
+      <c r="GX7" s="6"/>
+      <c r="GY7" s="6"/>
+      <c r="GZ7" s="6"/>
+      <c r="HA7" s="6"/>
+      <c r="HB7" s="6"/>
+      <c r="HC7" s="6"/>
+      <c r="HD7" s="6"/>
+      <c r="HE7" s="6"/>
+      <c r="HF7" s="6"/>
+      <c r="HG7" s="6"/>
+      <c r="HH7" s="6"/>
+      <c r="HI7" s="6"/>
+      <c r="HJ7" s="6"/>
+      <c r="HK7" s="6"/>
+      <c r="HL7" s="6"/>
+      <c r="HM7" s="6"/>
+      <c r="HN7" s="6"/>
+      <c r="HO7" s="6"/>
+      <c r="HP7" s="6"/>
+    </row>
+    <row r="8" spans="1:224" s="5" customFormat="1">
+      <c r="A8" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="6"/>
@@ -1376,14 +2858,212 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-    </row>
-    <row r="9" spans="1:26" s="5" customFormat="1">
-      <c r="A9" s="20" t="s">
-        <v>17</v>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="6"/>
+      <c r="AP8" s="6"/>
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="6"/>
+      <c r="AS8" s="6"/>
+      <c r="AT8" s="6"/>
+      <c r="AU8" s="6"/>
+      <c r="AV8" s="6"/>
+      <c r="AW8" s="6"/>
+      <c r="AX8" s="6"/>
+      <c r="AY8" s="6"/>
+      <c r="AZ8" s="6"/>
+      <c r="BA8" s="6"/>
+      <c r="BB8" s="6"/>
+      <c r="BC8" s="6"/>
+      <c r="BD8" s="6"/>
+      <c r="BE8" s="6"/>
+      <c r="BF8" s="6"/>
+      <c r="BG8" s="6"/>
+      <c r="BH8" s="6"/>
+      <c r="BI8" s="6"/>
+      <c r="BJ8" s="6"/>
+      <c r="BK8" s="6"/>
+      <c r="BL8" s="6"/>
+      <c r="BM8" s="6"/>
+      <c r="BN8" s="6"/>
+      <c r="BO8" s="6"/>
+      <c r="BP8" s="6"/>
+      <c r="BQ8" s="6"/>
+      <c r="BR8" s="6"/>
+      <c r="BS8" s="6"/>
+      <c r="BT8" s="6"/>
+      <c r="BU8" s="6"/>
+      <c r="BV8" s="6"/>
+      <c r="BW8" s="6"/>
+      <c r="BX8" s="6"/>
+      <c r="BY8" s="6"/>
+      <c r="BZ8" s="6"/>
+      <c r="CA8" s="6"/>
+      <c r="CB8" s="6"/>
+      <c r="CC8" s="6"/>
+      <c r="CD8" s="6"/>
+      <c r="CE8" s="6"/>
+      <c r="CF8" s="6"/>
+      <c r="CG8" s="6"/>
+      <c r="CH8" s="6"/>
+      <c r="CI8" s="6"/>
+      <c r="CJ8" s="6"/>
+      <c r="CK8" s="6"/>
+      <c r="CL8" s="6"/>
+      <c r="CM8" s="6"/>
+      <c r="CN8" s="6"/>
+      <c r="CO8" s="6"/>
+      <c r="CP8" s="6"/>
+      <c r="CQ8" s="6"/>
+      <c r="CR8" s="6"/>
+      <c r="CS8" s="6"/>
+      <c r="CT8" s="6"/>
+      <c r="CU8" s="6"/>
+      <c r="CV8" s="6"/>
+      <c r="CW8" s="6"/>
+      <c r="CX8" s="6"/>
+      <c r="CY8" s="6"/>
+      <c r="CZ8" s="6"/>
+      <c r="DA8" s="6"/>
+      <c r="DB8" s="6"/>
+      <c r="DC8" s="6"/>
+      <c r="DD8" s="6"/>
+      <c r="DE8" s="6"/>
+      <c r="DF8" s="6"/>
+      <c r="DG8" s="6"/>
+      <c r="DH8" s="6"/>
+      <c r="DI8" s="6"/>
+      <c r="DJ8" s="6"/>
+      <c r="DK8" s="6"/>
+      <c r="DL8" s="6"/>
+      <c r="DM8" s="6"/>
+      <c r="DN8" s="6"/>
+      <c r="DO8" s="6"/>
+      <c r="DP8" s="6"/>
+      <c r="DQ8" s="6"/>
+      <c r="DR8" s="6"/>
+      <c r="DS8" s="6"/>
+      <c r="DT8" s="6"/>
+      <c r="DU8" s="6"/>
+      <c r="DV8" s="6"/>
+      <c r="DW8" s="6"/>
+      <c r="DX8" s="6"/>
+      <c r="DY8" s="6"/>
+      <c r="DZ8" s="6"/>
+      <c r="EA8" s="6"/>
+      <c r="EB8" s="6"/>
+      <c r="EC8" s="6"/>
+      <c r="ED8" s="6"/>
+      <c r="EE8" s="6"/>
+      <c r="EF8" s="6"/>
+      <c r="EG8" s="6"/>
+      <c r="EH8" s="6"/>
+      <c r="EI8" s="6"/>
+      <c r="EJ8" s="6"/>
+      <c r="EK8" s="6"/>
+      <c r="EL8" s="6"/>
+      <c r="EM8" s="6"/>
+      <c r="EN8" s="6"/>
+      <c r="EO8" s="6"/>
+      <c r="EP8" s="6"/>
+      <c r="EQ8" s="6"/>
+      <c r="ER8" s="6"/>
+      <c r="ES8" s="6"/>
+      <c r="ET8" s="6"/>
+      <c r="EU8" s="6"/>
+      <c r="EV8" s="6"/>
+      <c r="EW8" s="6"/>
+      <c r="EX8" s="6"/>
+      <c r="EY8" s="6"/>
+      <c r="EZ8" s="6"/>
+      <c r="FA8" s="6"/>
+      <c r="FB8" s="6"/>
+      <c r="FC8" s="6"/>
+      <c r="FD8" s="6"/>
+      <c r="FE8" s="6"/>
+      <c r="FF8" s="6"/>
+      <c r="FG8" s="6"/>
+      <c r="FH8" s="6"/>
+      <c r="FI8" s="6"/>
+      <c r="FJ8" s="6"/>
+      <c r="FK8" s="6"/>
+      <c r="FL8" s="6"/>
+      <c r="FM8" s="6"/>
+      <c r="FN8" s="6"/>
+      <c r="FO8" s="6"/>
+      <c r="FP8" s="6"/>
+      <c r="FQ8" s="6"/>
+      <c r="FR8" s="6"/>
+      <c r="FS8" s="6"/>
+      <c r="FT8" s="6"/>
+      <c r="FU8" s="6"/>
+      <c r="FV8" s="6"/>
+      <c r="FW8" s="6"/>
+      <c r="FX8" s="6"/>
+      <c r="FY8" s="6"/>
+      <c r="FZ8" s="6"/>
+      <c r="GA8" s="6"/>
+      <c r="GB8" s="6"/>
+      <c r="GC8" s="6"/>
+      <c r="GD8" s="6"/>
+      <c r="GE8" s="6"/>
+      <c r="GF8" s="6"/>
+      <c r="GG8" s="6"/>
+      <c r="GH8" s="6"/>
+      <c r="GI8" s="6"/>
+      <c r="GJ8" s="6"/>
+      <c r="GK8" s="6"/>
+      <c r="GL8" s="6"/>
+      <c r="GM8" s="6"/>
+      <c r="GN8" s="6"/>
+      <c r="GO8" s="6"/>
+      <c r="GP8" s="6"/>
+      <c r="GQ8" s="6"/>
+      <c r="GR8" s="6"/>
+      <c r="GS8" s="6"/>
+      <c r="GT8" s="6"/>
+      <c r="GU8" s="6"/>
+      <c r="GV8" s="6"/>
+      <c r="GW8" s="6"/>
+      <c r="GX8" s="6"/>
+      <c r="GY8" s="6"/>
+      <c r="GZ8" s="6"/>
+      <c r="HA8" s="6"/>
+      <c r="HB8" s="6"/>
+      <c r="HC8" s="6"/>
+      <c r="HD8" s="6"/>
+      <c r="HE8" s="6"/>
+      <c r="HF8" s="6"/>
+      <c r="HG8" s="6"/>
+      <c r="HH8" s="6"/>
+      <c r="HI8" s="6"/>
+      <c r="HJ8" s="6"/>
+      <c r="HK8" s="6"/>
+      <c r="HL8" s="6"/>
+      <c r="HM8" s="6"/>
+      <c r="HN8" s="6"/>
+      <c r="HO8" s="6"/>
+      <c r="HP8" s="6"/>
+    </row>
+    <row r="9" spans="1:224" s="5" customFormat="1">
+      <c r="A9" s="19" t="s">
+        <v>15</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="6"/>
@@ -1408,14 +3088,212 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" s="5" customFormat="1">
-      <c r="A10" s="21" t="s">
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="6"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="6"/>
+      <c r="AP9" s="6"/>
+      <c r="AQ9" s="6"/>
+      <c r="AR9" s="6"/>
+      <c r="AS9" s="6"/>
+      <c r="AT9" s="6"/>
+      <c r="AU9" s="6"/>
+      <c r="AV9" s="6"/>
+      <c r="AW9" s="6"/>
+      <c r="AX9" s="6"/>
+      <c r="AY9" s="6"/>
+      <c r="AZ9" s="6"/>
+      <c r="BA9" s="6"/>
+      <c r="BB9" s="6"/>
+      <c r="BC9" s="6"/>
+      <c r="BD9" s="6"/>
+      <c r="BE9" s="6"/>
+      <c r="BF9" s="6"/>
+      <c r="BG9" s="6"/>
+      <c r="BH9" s="6"/>
+      <c r="BI9" s="6"/>
+      <c r="BJ9" s="6"/>
+      <c r="BK9" s="6"/>
+      <c r="BL9" s="6"/>
+      <c r="BM9" s="6"/>
+      <c r="BN9" s="6"/>
+      <c r="BO9" s="6"/>
+      <c r="BP9" s="6"/>
+      <c r="BQ9" s="6"/>
+      <c r="BR9" s="6"/>
+      <c r="BS9" s="6"/>
+      <c r="BT9" s="6"/>
+      <c r="BU9" s="6"/>
+      <c r="BV9" s="6"/>
+      <c r="BW9" s="6"/>
+      <c r="BX9" s="6"/>
+      <c r="BY9" s="6"/>
+      <c r="BZ9" s="6"/>
+      <c r="CA9" s="6"/>
+      <c r="CB9" s="6"/>
+      <c r="CC9" s="6"/>
+      <c r="CD9" s="6"/>
+      <c r="CE9" s="6"/>
+      <c r="CF9" s="6"/>
+      <c r="CG9" s="6"/>
+      <c r="CH9" s="6"/>
+      <c r="CI9" s="6"/>
+      <c r="CJ9" s="6"/>
+      <c r="CK9" s="6"/>
+      <c r="CL9" s="6"/>
+      <c r="CM9" s="6"/>
+      <c r="CN9" s="6"/>
+      <c r="CO9" s="6"/>
+      <c r="CP9" s="6"/>
+      <c r="CQ9" s="6"/>
+      <c r="CR9" s="6"/>
+      <c r="CS9" s="6"/>
+      <c r="CT9" s="6"/>
+      <c r="CU9" s="6"/>
+      <c r="CV9" s="6"/>
+      <c r="CW9" s="6"/>
+      <c r="CX9" s="6"/>
+      <c r="CY9" s="6"/>
+      <c r="CZ9" s="6"/>
+      <c r="DA9" s="6"/>
+      <c r="DB9" s="6"/>
+      <c r="DC9" s="6"/>
+      <c r="DD9" s="6"/>
+      <c r="DE9" s="6"/>
+      <c r="DF9" s="6"/>
+      <c r="DG9" s="6"/>
+      <c r="DH9" s="6"/>
+      <c r="DI9" s="6"/>
+      <c r="DJ9" s="6"/>
+      <c r="DK9" s="6"/>
+      <c r="DL9" s="6"/>
+      <c r="DM9" s="6"/>
+      <c r="DN9" s="6"/>
+      <c r="DO9" s="6"/>
+      <c r="DP9" s="6"/>
+      <c r="DQ9" s="6"/>
+      <c r="DR9" s="6"/>
+      <c r="DS9" s="6"/>
+      <c r="DT9" s="6"/>
+      <c r="DU9" s="6"/>
+      <c r="DV9" s="6"/>
+      <c r="DW9" s="6"/>
+      <c r="DX9" s="6"/>
+      <c r="DY9" s="6"/>
+      <c r="DZ9" s="6"/>
+      <c r="EA9" s="6"/>
+      <c r="EB9" s="6"/>
+      <c r="EC9" s="6"/>
+      <c r="ED9" s="6"/>
+      <c r="EE9" s="6"/>
+      <c r="EF9" s="6"/>
+      <c r="EG9" s="6"/>
+      <c r="EH9" s="6"/>
+      <c r="EI9" s="6"/>
+      <c r="EJ9" s="6"/>
+      <c r="EK9" s="6"/>
+      <c r="EL9" s="6"/>
+      <c r="EM9" s="6"/>
+      <c r="EN9" s="6"/>
+      <c r="EO9" s="6"/>
+      <c r="EP9" s="6"/>
+      <c r="EQ9" s="6"/>
+      <c r="ER9" s="6"/>
+      <c r="ES9" s="6"/>
+      <c r="ET9" s="6"/>
+      <c r="EU9" s="6"/>
+      <c r="EV9" s="6"/>
+      <c r="EW9" s="6"/>
+      <c r="EX9" s="6"/>
+      <c r="EY9" s="6"/>
+      <c r="EZ9" s="6"/>
+      <c r="FA9" s="6"/>
+      <c r="FB9" s="6"/>
+      <c r="FC9" s="6"/>
+      <c r="FD9" s="6"/>
+      <c r="FE9" s="6"/>
+      <c r="FF9" s="6"/>
+      <c r="FG9" s="6"/>
+      <c r="FH9" s="6"/>
+      <c r="FI9" s="6"/>
+      <c r="FJ9" s="6"/>
+      <c r="FK9" s="6"/>
+      <c r="FL9" s="6"/>
+      <c r="FM9" s="6"/>
+      <c r="FN9" s="6"/>
+      <c r="FO9" s="6"/>
+      <c r="FP9" s="6"/>
+      <c r="FQ9" s="6"/>
+      <c r="FR9" s="6"/>
+      <c r="FS9" s="6"/>
+      <c r="FT9" s="6"/>
+      <c r="FU9" s="6"/>
+      <c r="FV9" s="6"/>
+      <c r="FW9" s="6"/>
+      <c r="FX9" s="6"/>
+      <c r="FY9" s="6"/>
+      <c r="FZ9" s="6"/>
+      <c r="GA9" s="6"/>
+      <c r="GB9" s="6"/>
+      <c r="GC9" s="6"/>
+      <c r="GD9" s="6"/>
+      <c r="GE9" s="6"/>
+      <c r="GF9" s="6"/>
+      <c r="GG9" s="6"/>
+      <c r="GH9" s="6"/>
+      <c r="GI9" s="6"/>
+      <c r="GJ9" s="6"/>
+      <c r="GK9" s="6"/>
+      <c r="GL9" s="6"/>
+      <c r="GM9" s="6"/>
+      <c r="GN9" s="6"/>
+      <c r="GO9" s="6"/>
+      <c r="GP9" s="6"/>
+      <c r="GQ9" s="6"/>
+      <c r="GR9" s="6"/>
+      <c r="GS9" s="6"/>
+      <c r="GT9" s="6"/>
+      <c r="GU9" s="6"/>
+      <c r="GV9" s="6"/>
+      <c r="GW9" s="6"/>
+      <c r="GX9" s="6"/>
+      <c r="GY9" s="6"/>
+      <c r="GZ9" s="6"/>
+      <c r="HA9" s="6"/>
+      <c r="HB9" s="6"/>
+      <c r="HC9" s="6"/>
+      <c r="HD9" s="6"/>
+      <c r="HE9" s="6"/>
+      <c r="HF9" s="6"/>
+      <c r="HG9" s="6"/>
+      <c r="HH9" s="6"/>
+      <c r="HI9" s="6"/>
+      <c r="HJ9" s="6"/>
+      <c r="HK9" s="6"/>
+      <c r="HL9" s="6"/>
+      <c r="HM9" s="6"/>
+      <c r="HN9" s="6"/>
+      <c r="HO9" s="6"/>
+      <c r="HP9" s="6"/>
+    </row>
+    <row r="10" spans="1:224" s="5" customFormat="1">
+      <c r="A10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="21" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="22" t="s">
-        <v>21</v>
       </c>
       <c r="D10" s="2">
         <v>0.01</v>
@@ -1442,18 +3320,216 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" s="3" customFormat="1" ht="14" customHeight="1">
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="6"/>
+      <c r="AL10" s="6"/>
+      <c r="AM10" s="6"/>
+      <c r="AN10" s="6"/>
+      <c r="AO10" s="6"/>
+      <c r="AP10" s="6"/>
+      <c r="AQ10" s="6"/>
+      <c r="AR10" s="6"/>
+      <c r="AS10" s="6"/>
+      <c r="AT10" s="6"/>
+      <c r="AU10" s="6"/>
+      <c r="AV10" s="6"/>
+      <c r="AW10" s="6"/>
+      <c r="AX10" s="6"/>
+      <c r="AY10" s="6"/>
+      <c r="AZ10" s="6"/>
+      <c r="BA10" s="6"/>
+      <c r="BB10" s="6"/>
+      <c r="BC10" s="6"/>
+      <c r="BD10" s="6"/>
+      <c r="BE10" s="6"/>
+      <c r="BF10" s="6"/>
+      <c r="BG10" s="6"/>
+      <c r="BH10" s="6"/>
+      <c r="BI10" s="6"/>
+      <c r="BJ10" s="6"/>
+      <c r="BK10" s="6"/>
+      <c r="BL10" s="6"/>
+      <c r="BM10" s="6"/>
+      <c r="BN10" s="6"/>
+      <c r="BO10" s="6"/>
+      <c r="BP10" s="6"/>
+      <c r="BQ10" s="6"/>
+      <c r="BR10" s="6"/>
+      <c r="BS10" s="6"/>
+      <c r="BT10" s="6"/>
+      <c r="BU10" s="6"/>
+      <c r="BV10" s="6"/>
+      <c r="BW10" s="6"/>
+      <c r="BX10" s="6"/>
+      <c r="BY10" s="6"/>
+      <c r="BZ10" s="6"/>
+      <c r="CA10" s="6"/>
+      <c r="CB10" s="6"/>
+      <c r="CC10" s="6"/>
+      <c r="CD10" s="6"/>
+      <c r="CE10" s="6"/>
+      <c r="CF10" s="6"/>
+      <c r="CG10" s="6"/>
+      <c r="CH10" s="6"/>
+      <c r="CI10" s="6"/>
+      <c r="CJ10" s="6"/>
+      <c r="CK10" s="6"/>
+      <c r="CL10" s="6"/>
+      <c r="CM10" s="6"/>
+      <c r="CN10" s="6"/>
+      <c r="CO10" s="6"/>
+      <c r="CP10" s="6"/>
+      <c r="CQ10" s="6"/>
+      <c r="CR10" s="6"/>
+      <c r="CS10" s="6"/>
+      <c r="CT10" s="6"/>
+      <c r="CU10" s="6"/>
+      <c r="CV10" s="6"/>
+      <c r="CW10" s="6"/>
+      <c r="CX10" s="6"/>
+      <c r="CY10" s="6"/>
+      <c r="CZ10" s="6"/>
+      <c r="DA10" s="6"/>
+      <c r="DB10" s="6"/>
+      <c r="DC10" s="6"/>
+      <c r="DD10" s="6"/>
+      <c r="DE10" s="6"/>
+      <c r="DF10" s="6"/>
+      <c r="DG10" s="6"/>
+      <c r="DH10" s="6"/>
+      <c r="DI10" s="6"/>
+      <c r="DJ10" s="6"/>
+      <c r="DK10" s="6"/>
+      <c r="DL10" s="6"/>
+      <c r="DM10" s="6"/>
+      <c r="DN10" s="6"/>
+      <c r="DO10" s="6"/>
+      <c r="DP10" s="6"/>
+      <c r="DQ10" s="6"/>
+      <c r="DR10" s="6"/>
+      <c r="DS10" s="6"/>
+      <c r="DT10" s="6"/>
+      <c r="DU10" s="6"/>
+      <c r="DV10" s="6"/>
+      <c r="DW10" s="6"/>
+      <c r="DX10" s="6"/>
+      <c r="DY10" s="6"/>
+      <c r="DZ10" s="6"/>
+      <c r="EA10" s="6"/>
+      <c r="EB10" s="6"/>
+      <c r="EC10" s="6"/>
+      <c r="ED10" s="6"/>
+      <c r="EE10" s="6"/>
+      <c r="EF10" s="6"/>
+      <c r="EG10" s="6"/>
+      <c r="EH10" s="6"/>
+      <c r="EI10" s="6"/>
+      <c r="EJ10" s="6"/>
+      <c r="EK10" s="6"/>
+      <c r="EL10" s="6"/>
+      <c r="EM10" s="6"/>
+      <c r="EN10" s="6"/>
+      <c r="EO10" s="6"/>
+      <c r="EP10" s="6"/>
+      <c r="EQ10" s="6"/>
+      <c r="ER10" s="6"/>
+      <c r="ES10" s="6"/>
+      <c r="ET10" s="6"/>
+      <c r="EU10" s="6"/>
+      <c r="EV10" s="6"/>
+      <c r="EW10" s="6"/>
+      <c r="EX10" s="6"/>
+      <c r="EY10" s="6"/>
+      <c r="EZ10" s="6"/>
+      <c r="FA10" s="6"/>
+      <c r="FB10" s="6"/>
+      <c r="FC10" s="6"/>
+      <c r="FD10" s="6"/>
+      <c r="FE10" s="6"/>
+      <c r="FF10" s="6"/>
+      <c r="FG10" s="6"/>
+      <c r="FH10" s="6"/>
+      <c r="FI10" s="6"/>
+      <c r="FJ10" s="6"/>
+      <c r="FK10" s="6"/>
+      <c r="FL10" s="6"/>
+      <c r="FM10" s="6"/>
+      <c r="FN10" s="6"/>
+      <c r="FO10" s="6"/>
+      <c r="FP10" s="6"/>
+      <c r="FQ10" s="6"/>
+      <c r="FR10" s="6"/>
+      <c r="FS10" s="6"/>
+      <c r="FT10" s="6"/>
+      <c r="FU10" s="6"/>
+      <c r="FV10" s="6"/>
+      <c r="FW10" s="6"/>
+      <c r="FX10" s="6"/>
+      <c r="FY10" s="6"/>
+      <c r="FZ10" s="6"/>
+      <c r="GA10" s="6"/>
+      <c r="GB10" s="6"/>
+      <c r="GC10" s="6"/>
+      <c r="GD10" s="6"/>
+      <c r="GE10" s="6"/>
+      <c r="GF10" s="6"/>
+      <c r="GG10" s="6"/>
+      <c r="GH10" s="6"/>
+      <c r="GI10" s="6"/>
+      <c r="GJ10" s="6"/>
+      <c r="GK10" s="6"/>
+      <c r="GL10" s="6"/>
+      <c r="GM10" s="6"/>
+      <c r="GN10" s="6"/>
+      <c r="GO10" s="6"/>
+      <c r="GP10" s="6"/>
+      <c r="GQ10" s="6"/>
+      <c r="GR10" s="6"/>
+      <c r="GS10" s="6"/>
+      <c r="GT10" s="6"/>
+      <c r="GU10" s="6"/>
+      <c r="GV10" s="6"/>
+      <c r="GW10" s="6"/>
+      <c r="GX10" s="6"/>
+      <c r="GY10" s="6"/>
+      <c r="GZ10" s="6"/>
+      <c r="HA10" s="6"/>
+      <c r="HB10" s="6"/>
+      <c r="HC10" s="6"/>
+      <c r="HD10" s="6"/>
+      <c r="HE10" s="6"/>
+      <c r="HF10" s="6"/>
+      <c r="HG10" s="6"/>
+      <c r="HH10" s="6"/>
+      <c r="HI10" s="6"/>
+      <c r="HJ10" s="6"/>
+      <c r="HK10" s="6"/>
+      <c r="HL10" s="6"/>
+      <c r="HM10" s="6"/>
+      <c r="HN10" s="6"/>
+      <c r="HO10" s="6"/>
+      <c r="HP10" s="6"/>
+    </row>
+    <row r="11" spans="1:224" s="3" customFormat="1" ht="14" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="28">
+        <v>40</v>
+      </c>
+      <c r="B11" s="27">
         <v>0.3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="27">
+        <v>40</v>
+      </c>
+      <c r="D11" s="26">
         <v>0.02</v>
       </c>
       <c r="G11" s="4"/>
@@ -1477,15 +3553,18 @@
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:224">
       <c r="A12" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="28">
+        <v>41</v>
+      </c>
+      <c r="B12" s="27">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" ht="23">
+      <c r="D12" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:224" ht="23">
       <c r="A13" s="8" t="s">
         <v>0</v>
       </c>
@@ -1494,25 +3573,25 @@
       </c>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:224">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:224">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2">
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:224">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2">
         <v>0.6</v>
@@ -1520,7 +3599,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17" s="2">
         <v>0.01</v>
@@ -1528,7 +3607,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2">
         <v>0.4</v>
@@ -1536,69 +3615,131 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="20" t="s">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="15"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="28">
+        <v>42</v>
+      </c>
+      <c r="B23" s="27">
         <v>0.01</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="28">
+        <v>41</v>
+      </c>
+      <c r="B24" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+    <row r="25" spans="1:2" ht="23">
+      <c r="A25" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
+      <c r="A27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
+      <c r="A29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="15"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="27"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="27">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1613,10 +3754,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1628,115 +3769,196 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="10" customFormat="1" ht="23">
-      <c r="A1" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>46</v>
+      <c r="C1" s="25" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="2"/>
+      <c r="A2" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.9</v>
+      <c r="A3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="A4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14">
         <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="A5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23">
-      <c r="A6" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="26" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="23">
+      <c r="A7" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="25" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="A8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2">
+    <row r="10" spans="1:3">
+      <c r="A10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2">
+    <row r="11" spans="1:3">
+      <c r="A11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="23">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+    <row r="12" spans="1:3">
+      <c r="A12" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="23">
+      <c r="A13" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>